<commit_message>
include FG pre-filteration by rdki
</commit_message>
<xml_diff>
--- a/db_mis.xlsx
+++ b/db_mis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3434" documentId="11_F25DC773A252ABDACC1048E8991D7BDE5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4DA3A86-B950-49E1-9A49-810E5DD7BD7D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" tabRatio="660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solvent_db" sheetId="6" r:id="rId1"/>
@@ -4105,7 +4105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -4132,9 +4132,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4418,24 +4416,24 @@
   <dimension ref="A1:R251"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A244" sqref="A244:XFD244"/>
+      <selection pane="bottomLeft" activeCell="D162" sqref="D162:F162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="14" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="44.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="53.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4491,7 +4489,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4538,7 +4536,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4588,7 +4586,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4638,7 +4636,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4738,7 +4736,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4788,7 +4786,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4838,7 +4836,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4885,7 +4883,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4935,7 +4933,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4982,7 +4980,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5032,7 +5030,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5079,7 +5077,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5129,7 +5127,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5179,7 +5177,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5229,7 +5227,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -5276,7 +5274,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5326,7 +5324,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -5376,7 +5374,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5426,7 +5424,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -5476,7 +5474,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5526,7 +5524,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -5573,7 +5571,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5623,7 +5621,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -5667,7 +5665,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5717,7 +5715,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -5767,7 +5765,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5817,7 +5815,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5867,7 +5865,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5914,7 +5912,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5964,7 +5962,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -6011,7 +6009,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -6061,7 +6059,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -6108,7 +6106,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -6158,7 +6156,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -6208,7 +6206,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -6258,7 +6256,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -6305,7 +6303,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -6355,7 +6353,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6408,7 +6406,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -6461,7 +6459,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6511,7 +6509,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -6561,7 +6559,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6611,7 +6609,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -6664,7 +6662,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -6711,7 +6709,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -6761,7 +6759,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -6811,7 +6809,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -6861,7 +6859,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -6908,7 +6906,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -6955,7 +6953,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -7005,7 +7003,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -7055,7 +7053,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -7105,7 +7103,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -7155,7 +7153,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -7205,7 +7203,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -7252,7 +7250,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -7302,7 +7300,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -7352,7 +7350,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -7402,7 +7400,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -7452,7 +7450,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -7502,7 +7500,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -7552,7 +7550,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -7602,7 +7600,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -7652,7 +7650,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -7702,7 +7700,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -7752,7 +7750,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -7802,7 +7800,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -7852,7 +7850,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -7902,7 +7900,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -7949,7 +7947,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -7996,7 +7994,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -8046,7 +8044,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -8096,7 +8094,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -8146,7 +8144,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -8193,7 +8191,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -8240,7 +8238,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -8287,7 +8285,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -8334,7 +8332,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -8381,7 +8379,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -8431,7 +8429,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -8481,7 +8479,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -8528,7 +8526,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -8578,7 +8576,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -8625,7 +8623,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -8675,7 +8673,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -8725,7 +8723,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -8772,7 +8770,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -8822,7 +8820,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -8875,7 +8873,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -8922,7 +8920,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -8972,7 +8970,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -9019,7 +9017,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -9072,7 +9070,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -9125,7 +9123,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -9172,7 +9170,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -9222,7 +9220,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -9269,7 +9267,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -9316,7 +9314,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -9366,7 +9364,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -9416,7 +9414,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -9463,7 +9461,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -9513,7 +9511,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -9563,7 +9561,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -9613,7 +9611,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -9666,7 +9664,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -9716,7 +9714,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -9766,7 +9764,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -9816,7 +9814,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -9866,7 +9864,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -9916,7 +9914,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -9966,7 +9964,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -10016,7 +10014,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -10066,7 +10064,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -10116,7 +10114,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -10163,7 +10161,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -10213,7 +10211,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -10260,7 +10258,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -10310,7 +10308,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -10360,7 +10358,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -10410,7 +10408,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -10457,7 +10455,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -10504,7 +10502,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -10551,7 +10549,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -10598,7 +10596,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -10648,7 +10646,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -10695,7 +10693,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -10745,7 +10743,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -10795,7 +10793,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -10842,7 +10840,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -10892,7 +10890,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -10939,7 +10937,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -10986,7 +10984,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -11033,7 +11031,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -11080,7 +11078,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="136" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -11130,7 +11128,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -11180,7 +11178,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -11230,7 +11228,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -11280,7 +11278,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -11330,7 +11328,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -11380,7 +11378,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -11430,7 +11428,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -11480,7 +11478,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -11527,7 +11525,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -11577,7 +11575,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -11627,7 +11625,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -11677,7 +11675,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -11727,7 +11725,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -11777,7 +11775,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -11827,7 +11825,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -11877,7 +11875,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -11927,7 +11925,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -11977,7 +11975,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -12027,7 +12025,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -12074,7 +12072,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -12124,7 +12122,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -12171,7 +12169,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -12221,7 +12219,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -12271,7 +12269,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -12321,7 +12319,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -12374,7 +12372,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -12427,7 +12425,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -12474,7 +12472,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -12522,7 +12520,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -12572,7 +12570,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -12622,7 +12620,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -12672,7 +12670,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -12722,7 +12720,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -12772,7 +12770,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -12822,7 +12820,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -12869,7 +12867,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -12916,7 +12914,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -12966,7 +12964,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -13013,7 +13011,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -13060,7 +13058,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -13110,7 +13108,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -13160,7 +13158,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -13210,7 +13208,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -13257,7 +13255,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -13307,7 +13305,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -13357,7 +13355,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -13407,7 +13405,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -13457,7 +13455,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -13504,7 +13502,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -13554,7 +13552,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -13604,7 +13602,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -13654,7 +13652,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -13704,7 +13702,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -13754,7 +13752,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -13804,7 +13802,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -13854,7 +13852,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -13901,7 +13899,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -13948,7 +13946,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -13995,7 +13993,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -14042,7 +14040,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -14089,7 +14087,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -14136,7 +14134,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -14183,7 +14181,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -14230,7 +14228,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -14280,7 +14278,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -14327,7 +14325,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -14377,7 +14375,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -14427,7 +14425,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -14474,7 +14472,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -14524,7 +14522,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -14574,7 +14572,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -14621,7 +14619,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -14668,7 +14666,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -14718,7 +14716,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -14765,7 +14763,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -14812,7 +14810,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -14859,7 +14857,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -14906,7 +14904,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -14956,7 +14954,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -15006,7 +15004,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -15056,7 +15054,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -15106,7 +15104,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -15156,7 +15154,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -15206,7 +15204,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -15256,7 +15254,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -15312,7 +15310,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -15362,7 +15360,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -15412,7 +15410,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -15459,7 +15457,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -15509,7 +15507,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -15559,7 +15557,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -15606,7 +15604,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -15656,7 +15654,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -15706,7 +15704,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -15753,7 +15751,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -15803,7 +15801,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -15853,7 +15851,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>232</v>
       </c>
@@ -15903,7 +15901,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -15953,7 +15951,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -16000,7 +15998,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -16050,7 +16048,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -16100,7 +16098,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -16150,7 +16148,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -16197,7 +16195,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -16247,7 +16245,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -16300,7 +16298,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -16350,7 +16348,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -16397,7 +16395,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="244" spans="1:17" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -16447,7 +16445,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -16497,7 +16495,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -16547,26 +16545,26 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A247" s="5">
         <v>246</v>
       </c>
       <c r="B247" t="s">
         <v>699</v>
       </c>
-      <c r="C247" s="22" t="s">
+      <c r="C247" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="D247" s="21">
+      <c r="D247" s="10">
         <v>15.2</v>
       </c>
-      <c r="E247" s="21">
+      <c r="E247" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F247" s="21">
+      <c r="F247" s="10">
         <v>14.7</v>
       </c>
-      <c r="G247" s="21">
+      <c r="G247" s="10">
         <v>96</v>
       </c>
       <c r="I247" s="10">
@@ -16597,26 +16595,26 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A248" s="11">
         <v>247</v>
       </c>
       <c r="B248" s="13" t="s">
         <v>703</v>
       </c>
-      <c r="C248" s="20" t="s">
+      <c r="C248" t="s">
         <v>704</v>
       </c>
-      <c r="D248" s="20">
+      <c r="D248">
         <v>19.7</v>
       </c>
-      <c r="E248" s="20">
+      <c r="E248">
         <v>15.6</v>
       </c>
-      <c r="F248" s="20">
+      <c r="F248">
         <v>11.2</v>
       </c>
-      <c r="G248" s="20">
+      <c r="G248">
         <v>82.394000000000005</v>
       </c>
       <c r="I248" s="10">
@@ -16647,26 +16645,26 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A249" s="5">
         <v>248</v>
       </c>
       <c r="B249" t="s">
         <v>710</v>
       </c>
-      <c r="C249" s="20" t="s">
+      <c r="C249" t="s">
         <v>709</v>
       </c>
-      <c r="D249" s="20">
+      <c r="D249">
         <v>15.1</v>
       </c>
-      <c r="E249" s="20">
+      <c r="E249">
         <v>3.2</v>
       </c>
-      <c r="F249" s="20">
+      <c r="F249">
         <v>3.2</v>
       </c>
-      <c r="G249" s="20">
+      <c r="G249">
         <v>140.9</v>
       </c>
       <c r="H249" s="14" t="s">
@@ -16697,26 +16695,26 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A250" s="11">
         <v>249</v>
       </c>
       <c r="B250" t="s">
         <v>712</v>
       </c>
-      <c r="C250" s="20" t="s">
+      <c r="C250" t="s">
         <v>711</v>
       </c>
-      <c r="D250" s="20">
+      <c r="D250">
         <v>14.8</v>
       </c>
-      <c r="E250" s="20">
+      <c r="E250">
         <v>4.3</v>
       </c>
-      <c r="F250" s="20">
+      <c r="F250">
         <v>5</v>
       </c>
-      <c r="G250" s="20">
+      <c r="G250">
         <v>119.1</v>
       </c>
       <c r="H250" s="14" t="s">
@@ -16750,7 +16748,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A251" s="5"/>
     </row>
   </sheetData>

</xml_diff>